<commit_message>
Finished exercises for chapter 5 and part of 6
</commit_message>
<xml_diff>
--- a/Tutorial 2/Chapter 6/Morningstar.xlsx
+++ b/Tutorial 2/Chapter 6/Morningstar.xlsx
@@ -1,20 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\howde\Documents\Repos\MGMT220\Tutorial 2\Chapter 6\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88103742-A660-48DA-B348-9AD90248CA8F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18192" windowHeight="12336"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17985" windowHeight="5768" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Estimates" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <definedNames>
+    <definedName name="Rating">Estimates!$B$2:$B$41</definedName>
+    <definedName name="Risk">Estimates!$C$2:$C$41</definedName>
+  </definedNames>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="57">
   <si>
     <t>Company</t>
   </si>
@@ -167,13 +178,31 @@
   </si>
   <si>
     <t xml:space="preserve">Morningstar Rating </t>
+  </si>
+  <si>
+    <t>Point Estimate</t>
+  </si>
+  <si>
+    <t>Proportion</t>
+  </si>
+  <si>
+    <t>&lt;= 2 Star</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>Risk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,6 +222,14 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -215,13 +252,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -282,7 +321,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -315,9 +354,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -350,6 +406,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -525,22 +598,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.53125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -551,7 +624,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -562,7 +635,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -573,7 +646,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -584,7 +657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -595,7 +668,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -606,7 +679,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -617,7 +690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -628,7 +701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -639,7 +712,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -650,7 +723,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -661,7 +734,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -672,7 +745,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
@@ -683,7 +756,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
@@ -694,7 +767,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
@@ -705,7 +778,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
@@ -716,7 +789,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
@@ -727,7 +800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
@@ -738,7 +811,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
@@ -749,7 +822,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -760,7 +833,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
@@ -771,7 +844,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
@@ -782,7 +855,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
@@ -793,7 +866,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
@@ -804,7 +877,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>27</v>
       </c>
@@ -815,7 +888,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
         <v>28</v>
       </c>
@@ -826,7 +899,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
         <v>29</v>
       </c>
@@ -837,7 +910,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
         <v>30</v>
       </c>
@@ -848,7 +921,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
         <v>31</v>
       </c>
@@ -859,7 +932,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
         <v>32</v>
       </c>
@@ -870,7 +943,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
         <v>33</v>
       </c>
@@ -881,7 +954,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
         <v>34</v>
       </c>
@@ -892,7 +965,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
         <v>35</v>
       </c>
@@ -903,7 +976,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A34" s="2" t="s">
         <v>36</v>
       </c>
@@ -914,7 +987,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
         <v>37</v>
       </c>
@@ -925,7 +998,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A36" s="2" t="s">
         <v>38</v>
       </c>
@@ -936,7 +1009,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A37" s="2" t="s">
         <v>39</v>
       </c>
@@ -947,7 +1020,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A38" s="2" t="s">
         <v>40</v>
       </c>
@@ -958,7 +1031,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A39" s="2" t="s">
         <v>41</v>
       </c>
@@ -969,7 +1042,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
         <v>42</v>
       </c>
@@ -980,7 +1053,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A41" s="2" t="s">
         <v>43</v>
       </c>
@@ -994,4 +1067,538 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{796B1392-90C7-4B7B-A53F-753F935E1B9C}">
+  <dimension ref="A1:H41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.53125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.06640625" customWidth="1"/>
+    <col min="5" max="5" width="12.9296875" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.53125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2">
+        <f>COUNTIF(Rating, "5 Star")</f>
+        <v>2</v>
+      </c>
+      <c r="G2" s="5">
+        <f>F2/F6</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <f>COUNTIF(Risk, "Above Average")</f>
+        <v>17</v>
+      </c>
+      <c r="G3" s="5">
+        <f>F3/F7</f>
+        <v>0.42499999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4">
+        <f>COUNTIF(Rating, "&lt;=2 Star")</f>
+        <v>8</v>
+      </c>
+      <c r="G4" s="5">
+        <f>F4/F6</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6">
+        <f>COUNTA(Rating)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7">
+        <f>COUNTA(Risk)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A25" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A32" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A33" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A34" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A35" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A36" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A37" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A38" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A39" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A41" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>